<commit_message>
fixing autogen colon bug - initial attempt
</commit_message>
<xml_diff>
--- a/TIMES-NZ/SyncLogs/SynchronizeLogAllEntries - tasks.xlsx
+++ b/TIMES-NZ/SyncLogs/SynchronizeLogAllEntries - tasks.xlsx
@@ -8,32 +8,50 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41">
   <si>
     <t>WorkbookName</t>
   </si>
   <si>
+    <t>VT_NI_OTH_V4.xlsx</t>
+  </si>
+  <si>
     <t>SysSettings.xlsx</t>
   </si>
   <si>
+    <t>VT_SI_OTH_V4.xlsx</t>
+  </si>
+  <si>
     <t>SheetName</t>
   </si>
   <si>
+    <t>RES</t>
+  </si>
+  <si>
     <t>Interpol_Extrapol_Defaults</t>
   </si>
   <si>
     <t>Type</t>
   </si>
   <si>
+    <t>Base</t>
+  </si>
+  <si>
     <t>SysSettings</t>
   </si>
   <si>
     <t>Scenario</t>
   </si>
   <si>
+    <t>BASE</t>
+  </si>
+  <si>
     <t>Attribute</t>
   </si>
   <si>
+    <t>ncap_life</t>
+  </si>
+  <si>
     <t>ACT_BND</t>
   </si>
   <si>
@@ -52,12 +70,18 @@
     <t>Message</t>
   </si>
   <si>
+    <t>column is not recognized or invalid</t>
+  </si>
+  <si>
     <t>The process filter generated no records</t>
   </si>
   <si>
     <t>CellAddress</t>
   </si>
   <si>
+    <t>2,8</t>
+  </si>
+  <si>
     <t>3,1</t>
   </si>
   <si>
@@ -79,6 +103,9 @@
     <t>TagType</t>
   </si>
   <si>
+    <t>FI_T</t>
+  </si>
+  <si>
     <t>TFM_INS</t>
   </si>
   <si>
@@ -91,6 +118,9 @@
     <t>ProcessFilter</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>{"pset_pn": "IMP*GZ", "pset_set": "IRE"}</t>
   </si>
   <si>
@@ -101,9 +131,6 @@
   </si>
   <si>
     <t>CommodityFilter</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
 </sst>
 </file>
@@ -268,7 +295,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView zoomScale="100" topLeftCell="A1" workbookViewId="0" showGridLines="true" showRowColHeaders="true" view="normal"/>
   </sheetViews>
@@ -279,34 +306,34 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="I1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="J1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="K1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2">
@@ -314,209 +341,279 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="J2" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="K2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="J3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="K3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="J4" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="K4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="J5" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K5" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="I6" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J6" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K6" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
         <v>3</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" t="s">
-        <v>28</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" t="s">
         <v>31</v>
+      </c>
+      <c r="J9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refreshed IAT and ensured test passed
</commit_message>
<xml_diff>
--- a/TIMES-NZ/SyncLogs/SynchronizeLogAllEntries - tasks.xlsx
+++ b/TIMES-NZ/SyncLogs/SynchronizeLogAllEntries - tasks.xlsx
@@ -8,27 +8,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53">
   <si>
     <t>WorkbookName</t>
   </si>
   <si>
+    <t>VT_SI_OTH_V4.xlsx</t>
+  </si>
+  <si>
+    <t>VT_NI_PRI_V4.xlsx</t>
+  </si>
+  <si>
+    <t>SysSettings.xlsx</t>
+  </si>
+  <si>
     <t>VT_NI_OTH_V4.xlsx</t>
   </si>
   <si>
-    <t>SysSettings.xlsx</t>
-  </si>
-  <si>
-    <t>VT_SI_OTH_V4.xlsx</t>
+    <t>VT_NI_TRA_V4.xlsx</t>
+  </si>
+  <si>
+    <t>VT_SI_TRA_V4.xlsx</t>
   </si>
   <si>
     <t>SheetName</t>
   </si>
   <si>
+    <t>COM</t>
+  </si>
+  <si>
+    <t>SUP_H2</t>
+  </si>
+  <si>
+    <t>Interpol_Extrapol_Defaults</t>
+  </si>
+  <si>
     <t>RES</t>
   </si>
   <si>
-    <t>Interpol_Extrapol_Defaults</t>
+    <t>TRA_FuelSupply</t>
+  </si>
+  <si>
+    <t>TRA_Demand-Vehicles</t>
   </si>
   <si>
     <t>Type</t>
@@ -49,18 +70,21 @@
     <t>Attribute</t>
   </si>
   <si>
+    <t>missing_colname_1</t>
+  </si>
+  <si>
+    <t>ACT_BND</t>
+  </si>
+  <si>
+    <t>PRC_TSL</t>
+  </si>
+  <si>
+    <t>ACTCOST</t>
+  </si>
+  <si>
     <t>ncap_life</t>
   </si>
   <si>
-    <t>ACT_BND</t>
-  </si>
-  <si>
-    <t>PRC_TSL</t>
-  </si>
-  <si>
-    <t>ACTCOST</t>
-  </si>
-  <si>
     <t>MessageCategory</t>
   </si>
   <si>
@@ -79,25 +103,37 @@
     <t>CellAddress</t>
   </si>
   <si>
-    <t>2,8</t>
-  </si>
-  <si>
-    <t>3,1</t>
-  </si>
-  <si>
-    <t>4,1</t>
-  </si>
-  <si>
-    <t>5,1</t>
-  </si>
-  <si>
-    <t>9,1</t>
-  </si>
-  <si>
-    <t>22,1</t>
-  </si>
-  <si>
-    <t>23,1</t>
+    <t>4,19</t>
+  </si>
+  <si>
+    <t>77,12</t>
+  </si>
+  <si>
+    <t>23,2</t>
+  </si>
+  <si>
+    <t>24,2</t>
+  </si>
+  <si>
+    <t>25,2</t>
+  </si>
+  <si>
+    <t>32,2</t>
+  </si>
+  <si>
+    <t>15,2</t>
+  </si>
+  <si>
+    <t>16,2</t>
+  </si>
+  <si>
+    <t>5,10</t>
+  </si>
+  <si>
+    <t>21,1</t>
+  </si>
+  <si>
+    <t>75,2</t>
   </si>
   <si>
     <t>TagType</t>
@@ -295,7 +331,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView zoomScale="100" topLeftCell="A1" workbookViewId="0" showGridLines="true" showRowColHeaders="true" view="normal"/>
   </sheetViews>
@@ -306,34 +342,34 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="H1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="I1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="J1" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="K1" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2">
@@ -341,34 +377,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="I2" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="J2" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="K2" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
@@ -376,209 +412,209 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="I3" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="J3" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="K3" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="J4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="K4" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="I5" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="J5" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="K5" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="J6" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="K6" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="I7" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="J7" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="K7" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="H8" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="I8" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="J8" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="K8" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9">
@@ -586,34 +622,209 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" t="s">
+        <v>48</v>
+      </c>
+      <c r="K11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" t="s">
+        <v>48</v>
+      </c>
+      <c r="K12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
         <v>5</v>
       </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="F9" t="s">
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
         <v>18</v>
       </c>
-      <c r="G9" t="s">
+      <c r="E14" t="s">
         <v>20</v>
       </c>
-      <c r="H9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" t="s">
-        <v>31</v>
-      </c>
-      <c r="J9" t="s">
-        <v>36</v>
-      </c>
-      <c r="K9" t="s">
-        <v>36</v>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K14" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>